<commit_message>
add the latest xml file (7.4)
</commit_message>
<xml_diff>
--- a/result_xlsx_files/teacher_time_table.xlsx
+++ b/result_xlsx_files/teacher_time_table.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="173">
   <si>
     <t>9.00-9.30</t>
   </si>
@@ -257,6 +257,10 @@
 Go Master</t>
   </si>
   <si>
+    <t>POSN Mathematics
+P'Aong</t>
+  </si>
+  <si>
     <t>9B English
 Mr.Jacob</t>
   </si>
@@ -311,14 +315,14 @@
 P'Amy</t>
   </si>
   <si>
+    <t>9 Chinese Intermediate
+P'Chai</t>
+  </si>
+  <si>
     <t>9D Mathematics
 P'Cee</t>
   </si>
   <si>
-    <t>9 Chinese Intermediate
-P'Chai</t>
-  </si>
-  <si>
     <t>9D GO
 Go Master</t>
   </si>
@@ -357,11 +361,32 @@
     <t>12NBS-A Character Development</t>
   </si>
   <si>
+    <t>12NBS-A Work Experience</t>
+  </si>
+  <si>
+    <t>12NBS-A Managing a Successful Business Project
+Mr.James</t>
+  </si>
+  <si>
+    <t>12NBS-A IELTS
+Mr.Marc</t>
+  </si>
+  <si>
+    <t>12NBS SAT Eng
+P'Umim</t>
+  </si>
+  <si>
+    <t>12NBS Semester 1 Units</t>
+  </si>
+  <si>
+    <t>12NBS Work Experience - Self Work</t>
+  </si>
+  <si>
     <t>12NBS-A Business Data and Numerical Skills
 P'Mint</t>
   </si>
   <si>
-    <t>12NBS-A Managing a Successful Business Project
+    <t>12NBS-A Business Project - Self work
 Mr.James</t>
   </si>
   <si>
@@ -369,28 +394,6 @@
 Mr.James</t>
   </si>
   <si>
-    <t>12NBS-A Business Data and Numerical Skills - Practicum
-P'Mint</t>
-  </si>
-  <si>
-    <t>12NBS-A IELTS
-Mr.Marc</t>
-  </si>
-  <si>
-    <t>12NBS SAT Eng
-P'Umim</t>
-  </si>
-  <si>
-    <t>12NBS Semester 1 Units</t>
-  </si>
-  <si>
-    <t>12NBS-A Business Project - Self work
-Mr.James</t>
-  </si>
-  <si>
-    <t>12NBS-A Work Experience</t>
-  </si>
-  <si>
     <t>12NBS-B Character Development</t>
   </si>
   <si>
@@ -401,10 +404,6 @@
 Mr.Marc</t>
   </si>
   <si>
-    <t>12NBS-B Business Data and Numerical Skills - Practicum
-P'Mint</t>
-  </si>
-  <si>
     <t>12NBS-B Managing a Successful Business Project
 P'Chua</t>
   </si>
@@ -420,33 +419,33 @@
     <t>13NBS Character Development</t>
   </si>
   <si>
+    <t>13 Business Strategy
+P'Mint</t>
+  </si>
+  <si>
+    <t>13NBS Unit 26 &amp; 33 OpsÂ MngmtÂ andÂ Mktg
+Mr.James</t>
+  </si>
+  <si>
     <t>13NBS Financial Management
 Ms.Shruti</t>
   </si>
   <si>
-    <t>13 Business Strategy
-P'Mint</t>
-  </si>
-  <si>
     <t>13NBS Financial Management - Practicum
 Ms.Shruti</t>
   </si>
   <si>
-    <t>13NBS Managing a Successful Business Project - Practicum
-Mr.James</t>
-  </si>
-  <si>
     <t>13NBS Organisational Behaviour</t>
+  </si>
+  <si>
+    <t>13Hum University Preparation / Activities
+P'Best</t>
   </si>
   <si>
     <t>13NBS IELTS
 Mr.Marc</t>
   </si>
   <si>
-    <t>13NBS Managing a Successful Business Project
-Mr.James</t>
-  </si>
-  <si>
     <t>12,13 Business Strategy</t>
   </si>
   <si>
@@ -468,21 +467,21 @@
     <t>10A Character Development</t>
   </si>
   <si>
+    <t>10A Chemistry
+P'Boom</t>
+  </si>
+  <si>
+    <t>10A Mathematics
+P'Korn</t>
+  </si>
+  <si>
+    <t>11 Academic Clinic</t>
+  </si>
+  <si>
     <t>10A English A
 Mr.Brian</t>
   </si>
   <si>
-    <t>10A Chemistry
-P'Boom</t>
-  </si>
-  <si>
-    <t>10A Mathematics
-P'Korn</t>
-  </si>
-  <si>
-    <t>11 Academic Clinic</t>
-  </si>
-  <si>
     <t>10 Academic Clinic</t>
   </si>
   <si>
@@ -493,8 +492,8 @@
 P'Namfon</t>
   </si>
   <si>
-    <t>10BC English A
-Mr.Aaron</t>
+    <t>POSN Chemistry
+P'Win</t>
   </si>
   <si>
     <t>11 Mock IGCSE</t>
@@ -515,11 +514,15 @@
 P'June</t>
   </si>
   <si>
+    <t>10C Physics
+P'Fluke</t>
+  </si>
+  <si>
     <t>10BC English as a second language
 P'Jay</t>
   </si>
   <si>
-    <t>10C Physics
+    <t>POSN Physics
 P'Fluke</t>
   </si>
   <si>
@@ -550,18 +553,21 @@
 P'Oho</t>
   </si>
   <si>
+    <t>10E Chemistry
+P'Win</t>
+  </si>
+  <si>
+    <t>10E Mathematics
+P'Sun</t>
+  </si>
+  <si>
+    <t>12 Mock A-Level</t>
+  </si>
+  <si>
     <t>10E Physics
 P'Cee</t>
   </si>
   <si>
-    <t>10E Chemistry
-P'Win</t>
-  </si>
-  <si>
-    <t>10E Mathematics
-P'Sun</t>
-  </si>
-  <si>
     <t>10DE English as a second language
 P'Yuri</t>
   </si>
@@ -591,46 +597,50 @@
     <t>12Med Portfolio and Research</t>
   </si>
   <si>
+    <t>11 SAT Eng
+P'Umim</t>
+  </si>
+  <si>
+    <t>13 Psychology
+Dr.Ae</t>
+  </si>
+  <si>
+    <t>12 IELTS by Ms.Sam
+Ms.Sam</t>
+  </si>
+  <si>
+    <t>12Med Mathematics
+P'June</t>
+  </si>
+  <si>
+    <t>12Med-A Character Development</t>
+  </si>
+  <si>
+    <t>12Com,13Com Project</t>
+  </si>
+  <si>
+    <t>12Med BMAT: Mathematics
+P'Aom</t>
+  </si>
+  <si>
+    <t>12 Justice and Leadership
+Mr.Brian</t>
+  </si>
+  <si>
+    <t>12Com SAT Eng
+P'Mook</t>
+  </si>
+  <si>
+    <t>12Com IELTS by P'Gib
+P'Gib</t>
+  </si>
+  <si>
+    <t>12Med BMAT Part 3: Writing Task
+P'Ya</t>
+  </si>
+  <si>
     <t>12Med BMAT: Biology
 P'Ya</t>
-  </si>
-  <si>
-    <t>11 SAT Eng
-P'Umim</t>
-  </si>
-  <si>
-    <t>13 Psychology
-Dr.Ae</t>
-  </si>
-  <si>
-    <t>12 IELTS by Ms.Sam
-Ms.Sam</t>
-  </si>
-  <si>
-    <t>12Med Mathematics
-P'June</t>
-  </si>
-  <si>
-    <t>12Med-A Character Development</t>
-  </si>
-  <si>
-    <t>12Com,13Com Project</t>
-  </si>
-  <si>
-    <t>12Med BMAT: Mathematics
-P'Aom</t>
-  </si>
-  <si>
-    <t>12 Justice and Leadership
-Mr.Brian</t>
-  </si>
-  <si>
-    <t>12Com IELTS by P'Gib
-P'Gib</t>
-  </si>
-  <si>
-    <t>12Com SAT Eng
-P'Gib</t>
   </si>
   <si>
     <t>12Com Mathematics
@@ -1845,16 +1855,14 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1862,24 +1870,17 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1900,7 +1901,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1914,11 +1915,11 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1929,25 +1930,27 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1957,16 +1960,12 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1977,18 +1976,15 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="13">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="D2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B4:C4"/>
@@ -1996,10 +1992,9 @@
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="L5:O5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
     <mergeCell ref="P6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2077,16 +2072,14 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2094,24 +2087,20 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2143,7 +2132,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -2170,7 +2159,9 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -2203,16 +2194,15 @@
       <c r="R6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="D2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="L5:O5"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2222,7 +2212,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2231,7 +2221,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="105" customHeight="1">
+    <row r="1" spans="1:20" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2285,7 +2275,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="105" customHeight="1">
+    <row r="2" spans="1:20" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -2306,46 +2296,49 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="105" customHeight="1">
+    <row r="3" spans="1:20" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="I3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" ht="105" customHeight="1">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2356,17 +2349,17 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="105" customHeight="1">
+    <row r="5" spans="1:20" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2379,11 +2372,11 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -2391,12 +2384,12 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="105" customHeight="1">
+    <row r="6" spans="1:20" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2419,13 +2412,13 @@
   <mergeCells count="12">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="L4:M4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="B6:C6"/>
@@ -2999,7 +2992,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3008,7 +3001,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="105" customHeight="1">
+    <row r="1" spans="1:21" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3062,7 +3055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="105" customHeight="1">
+    <row r="2" spans="1:21" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3072,32 +3065,30 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="105" customHeight="1">
+    <row r="3" spans="1:21" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -3107,7 +3098,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -3115,16 +3106,18 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="105" customHeight="1">
+    <row r="4" spans="1:21" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -3133,7 +3126,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -3144,12 +3137,12 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:20" ht="105" customHeight="1">
+    <row r="5" spans="1:21" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3162,21 +3155,21 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="O5" s="1"/>
-      <c r="P5" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" ht="105" customHeight="1">
+    </row>
+    <row r="6" spans="1:21" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3184,37 +3177,37 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="P6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="S6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="R3:S3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="S6:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -3404,7 +3397,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3413,7 +3406,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="105" customHeight="1">
+    <row r="1" spans="1:19" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3467,7 +3460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="105" customHeight="1">
+    <row r="2" spans="1:19" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3489,11 +3482,14 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" ht="105" customHeight="1">
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -3503,9 +3499,7 @@
         <v>121</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3521,15 +3515,13 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="105" customHeight="1">
+    <row r="4" spans="1:19" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -3545,23 +3537,21 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="105" customHeight="1">
+    <row r="5" spans="1:19" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -3571,13 +3561,11 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="105" customHeight="1">
+    <row r="6" spans="1:19" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3585,33 +3573,30 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="8">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="P6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -3620,7 +3605,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3629,7 +3614,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="105" customHeight="1">
+    <row r="1" spans="1:23" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3683,7 +3668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="105" customHeight="1">
+    <row r="2" spans="1:23" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3713,59 +3698,58 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="105" customHeight="1">
+    <row r="3" spans="1:23" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="1:21" ht="105" customHeight="1">
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:23" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -3773,9 +3757,8 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" ht="105" customHeight="1">
+    </row>
+    <row r="5" spans="1:23" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -3784,7 +3767,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3800,11 +3783,14 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" ht="105" customHeight="1">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -3812,58 +3798,57 @@
         <v>129</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="R6" s="1"/>
-      <c r="S6" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
+      <c r="U6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M3:P3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="I5:L5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="U6:V6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -3942,11 +3927,11 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3963,29 +3948,38 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:19" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3994,44 +3988,40 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4039,12 +4029,12 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -4054,15 +4044,16 @@
       <c r="S6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="I5:L5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="J6:K6"/>
@@ -4075,7 +4066,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4084,7 +4075,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="105" customHeight="1">
+    <row r="1" spans="1:19" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4138,14 +4129,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="105" customHeight="1">
+    <row r="2" spans="1:19" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -4155,7 +4146,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -4164,33 +4155,33 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="105" customHeight="1">
+    <row r="3" spans="1:19" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="105" customHeight="1">
+    <row r="4" spans="1:19" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -4201,7 +4192,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -4215,16 +4206,16 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:20" ht="105" customHeight="1">
+    <row r="5" spans="1:19" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4234,7 +4225,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -4243,55 +4234,52 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" ht="105" customHeight="1">
+    </row>
+    <row r="6" spans="1:19" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:G6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -4370,7 +4358,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -4406,7 +4394,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -4416,7 +4404,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4430,7 +4418,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -4579,7 +4567,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -4603,7 +4591,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -4649,7 +4637,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -4761,7 +4749,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -4769,7 +4757,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -4803,9 +4791,7 @@
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -4816,7 +4802,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -4838,7 +4824,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -4854,7 +4840,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -4864,7 +4850,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -4876,10 +4862,9 @@
       <c r="R6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="B6:C6"/>
@@ -5140,7 +5125,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5154,7 +5139,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -5166,7 +5151,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -5178,7 +5163,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -5199,9 +5184,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
         <v>158</v>
@@ -5217,13 +5200,15 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -5243,14 +5228,18 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -5262,14 +5251,16 @@
       <c r="R6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="J6:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5761,7 +5752,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -5771,7 +5762,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -5795,7 +5786,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -5819,7 +5810,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -5843,7 +5834,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -5967,7 +5958,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -5991,7 +5982,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -6015,7 +6006,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -6039,7 +6030,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -6184,7 +6175,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -6721,7 +6712,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6730,7 +6721,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="105" customHeight="1">
+    <row r="1" spans="1:21" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -6784,7 +6775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="105" customHeight="1">
+    <row r="2" spans="1:21" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -6810,7 +6801,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="105" customHeight="1">
+    <row r="3" spans="1:21" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -6834,19 +6825,22 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:22" ht="105" customHeight="1">
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -6859,7 +6853,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -6869,12 +6863,12 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="105" customHeight="1">
+    <row r="5" spans="1:21" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -6895,7 +6889,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="105" customHeight="1">
+    <row r="6" spans="1:21" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -6907,7 +6901,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -6916,18 +6910,15 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -6937,6 +6928,7 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="I4:J4"/>
@@ -6945,7 +6937,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="O6:P6"/>
     <mergeCell ref="Q6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7023,11 +7014,11 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -7035,7 +7026,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -7044,7 +7035,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -7055,26 +7046,26 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -7087,13 +7078,13 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -7101,12 +7092,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -7117,14 +7108,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -7145,11 +7136,11 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -7157,13 +7148,13 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -7267,24 +7258,22 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -7296,7 +7285,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -7308,7 +7297,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -7317,7 +7306,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -7328,15 +7317,15 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -7354,7 +7343,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
@@ -7380,21 +7369,21 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -7406,11 +7395,10 @@
       <c r="R6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:M2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:M3"/>
@@ -7432,7 +7420,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7441,7 +7429,7 @@
     <col min="1" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="105" customHeight="1">
+    <row r="1" spans="1:21" ht="105" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -7495,16 +7483,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="105" customHeight="1">
+    <row r="2" spans="1:21" ht="105" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -7520,23 +7508,23 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="105" customHeight="1">
+    <row r="3" spans="1:21" ht="105" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -7545,32 +7533,32 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="105" customHeight="1">
+    <row r="4" spans="1:21" ht="105" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -7581,12 +7569,12 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="105" customHeight="1">
+    <row r="5" spans="1:21" ht="105" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -7594,48 +7582,51 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" ht="105" customHeight="1">
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="105" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -7651,7 +7642,7 @@
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L5:O5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="I6:J6"/>

</xml_diff>